<commit_message>
Adding changes to the donations page . Improvised method to read excel by page type in common methods.
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poonamwadkar/Documents/ESFA_Repositories/AcademyAccountReturn/AR2_3/src/test/resources/DATA_SHEETS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poonamwadkar/Documents/ESFA_Repositories/AcademyAccountReturn/AR2_3/src/test/dataSheetsResources/AR_DataSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Donations" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,31 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>IFC3 - Additions (£000)</t>
   </si>
@@ -82,13 +59,61 @@
   </si>
   <si>
     <t>IFC12 - At close of period (£000)</t>
+  </si>
+  <si>
+    <t>D1 - Donated Fixed Assets - DfE and ESFA (EFA)   </t>
+  </si>
+  <si>
+    <t>D2 - Donated Fixed Assets (Non-DfE and ESFA (EFA))   </t>
+  </si>
+  <si>
+    <t>D3 - Donated Intangible Assets  </t>
+  </si>
+  <si>
+    <t>D4 - Other Donations (Capital)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5 - Total Capital </t>
+  </si>
+  <si>
+    <t>D6 - Other Donations (Revenue)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7 - Total Revenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8 - Total </t>
+  </si>
+  <si>
+    <t>D1 - Donated Fixed Assets - DfE and ESFA (EFA)</t>
+  </si>
+  <si>
+    <t>D2 - Donated Fixed Assets (Non-DfE and ESFA (EFA))</t>
+  </si>
+  <si>
+    <t>D3 - Donated Intangible Assets </t>
+  </si>
+  <si>
+    <t>D4 - Other Donations (Capital)</t>
+  </si>
+  <si>
+    <t>D5 - Total Capital</t>
+  </si>
+  <si>
+    <t>D6 - Other Donations (Revenue)</t>
+  </si>
+  <si>
+    <t>D7 - Total Revenue</t>
+  </si>
+  <si>
+    <t>D8 - Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +140,29 @@
       <name val="Andale Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0B0C0C"/>
+      <name val="Andale Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,16 +181,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,50 +480,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -473,9 +536,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -486,61 +608,61 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>

</xml_diff>

<commit_message>
Adding new references to the excel sheet
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="920" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="13" activeTab="22"/>
+    <workbookView xWindow="-20" yWindow="920" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="43" activeTab="52"/>
   </bookViews>
   <sheets>
     <sheet name="s_Donations" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,41 @@
     <sheet name="s_st_OffPayrollArr" sheetId="23" r:id="rId21"/>
     <sheet name="s_pba_Income" sheetId="24" r:id="rId22"/>
     <sheet name="s_pba_Exp" sheetId="25" r:id="rId23"/>
+    <sheet name="bsa_ifa_Cost" sheetId="26" r:id="rId24"/>
+    <sheet name="bsa_ifa_Amortisation" sheetId="27" r:id="rId25"/>
+    <sheet name="bsa_ifa_Impairments" sheetId="28" r:id="rId26"/>
+    <sheet name="bsa_ifa_NetBookValue" sheetId="29" r:id="rId27"/>
+    <sheet name="bsa_ifa_AssetFinancing" sheetId="30" r:id="rId28"/>
+    <sheet name="bsa_ifa_AmortisationPeriods" sheetId="31" r:id="rId29"/>
+    <sheet name="bsa_nci" sheetId="32" r:id="rId30"/>
+    <sheet name="bsa_ci" sheetId="33" r:id="rId31"/>
+    <sheet name="bsa_tfa_Cost" sheetId="34" r:id="rId32"/>
+    <sheet name="bsa_tfa_Depriciation" sheetId="35" r:id="rId33"/>
+    <sheet name="bsa_tfa_Impairments" sheetId="36" r:id="rId34"/>
+    <sheet name="bsa_tfa_NetBookValue" sheetId="37" r:id="rId35"/>
+    <sheet name="bsa_tfa_AssetsFinancing" sheetId="38" r:id="rId36"/>
+    <sheet name="bsa_tfa_DepriciationPeriods" sheetId="39" r:id="rId37"/>
+    <sheet name="bsa_Debtors" sheetId="40" r:id="rId38"/>
+    <sheet name="bsa_Cash" sheetId="42" r:id="rId39"/>
+    <sheet name="auc_CapitalGrants" sheetId="43" r:id="rId40"/>
+    <sheet name="auc_Donations" sheetId="44" r:id="rId41"/>
+    <sheet name="auc_Transfers" sheetId="50" r:id="rId42"/>
+    <sheet name="auc_tfa_Cost" sheetId="45" r:id="rId43"/>
+    <sheet name="auc_tfa_Depriciation" sheetId="46" r:id="rId44"/>
+    <sheet name="auc_tfa_Impairments" sheetId="47" r:id="rId45"/>
+    <sheet name="auc_Debtors" sheetId="48" r:id="rId46"/>
+    <sheet name="auc_Other" sheetId="49" r:id="rId47"/>
+    <sheet name="lnb_to_Cost" sheetId="51" r:id="rId48"/>
+    <sheet name="lnb_to_Depriciation" sheetId="52" r:id="rId49"/>
+    <sheet name="lnb_lnbt_Cost" sheetId="53" r:id="rId50"/>
+    <sheet name="lnb_lnbt_Depriciation" sheetId="58" r:id="rId51"/>
+    <sheet name="lnb_lnbt_Impairment" sheetId="59" r:id="rId52"/>
+    <sheet name="lnb_lnbt_NetBookValue" sheetId="60" r:id="rId53"/>
+    <sheet name="lnb_to_Impairment" sheetId="54" r:id="rId54"/>
+    <sheet name="lnb_a_Cost" sheetId="55" r:id="rId55"/>
+    <sheet name="lnb_a_Depriciation" sheetId="56" r:id="rId56"/>
+    <sheet name="lnb_a_Impairment" sheetId="57" r:id="rId57"/>
+    <sheet name="bsa_Stock" sheetId="41" r:id="rId58"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -49,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="603">
   <si>
     <t>D1 - Donated Fixed Assets - DfE and ESFA (EFA)</t>
   </si>
@@ -913,6 +948,951 @@
   </si>
   <si>
     <t>Value of Arrangements (£000) - B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Original prior year closing balance (£000) - IFC1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - IFC2</t>
+  </si>
+  <si>
+    <t>Additions (£000) - IFC3</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - IFC4</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - IFC5</t>
+  </si>
+  <si>
+    <t>Transferred in on existing academies joining the trust (£000) - IFC6</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - IFC7</t>
+  </si>
+  <si>
+    <t>Donations (£000) - IFC8</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - IFC9</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - IFC10</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - IFC11</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - IFC12</t>
+  </si>
+  <si>
+    <t>Software - A</t>
+  </si>
+  <si>
+    <t>Other - B</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - IFA1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - IFA2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - IFA3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - IFA4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - IFA5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - IFA6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - IFA7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - IFA8</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - IFA9</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - IFI1</t>
+  </si>
+  <si>
+    <t>Other Adjustments made to opening balance (£000) - IFI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - IFI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - IFI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - IFI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - IFI6</t>
+  </si>
+  <si>
+    <t>Closing Balance (£000) - IFI7</t>
+  </si>
+  <si>
+    <t>Closing net book value (£000) - IFV1</t>
+  </si>
+  <si>
+    <t>Software - IFV2</t>
+  </si>
+  <si>
+    <t>Other  - IFV3</t>
+  </si>
+  <si>
+    <t>Total  - IFV4</t>
+  </si>
+  <si>
+    <t>Owned (£000) - IFF1</t>
+  </si>
+  <si>
+    <t>Finance leased (£000) - IFF2</t>
+  </si>
+  <si>
+    <t>On-balance sheet PFI contracts (£000) - IFF3</t>
+  </si>
+  <si>
+    <t>Closing net book value (£000) - IFF4</t>
+  </si>
+  <si>
+    <t>missing ref numbers in specification</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - NCI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - NCI2</t>
+  </si>
+  <si>
+    <t>Additions (£000) - NCI3</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - NCI4</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - NCI5</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - NCI6</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - NCI7</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - NCI8</t>
+  </si>
+  <si>
+    <t>Impairments (£000) - NCI9</t>
+  </si>
+  <si>
+    <t>Reclassification from current asset investments (£000) - NCI10</t>
+  </si>
+  <si>
+    <t>Reclassification to current asset investments (£000) - NCI11</t>
+  </si>
+  <si>
+    <t>Reclassification within non current investments (£000) - NCI12</t>
+  </si>
+  <si>
+    <t>Period end fair value gain/(loss) (£000) - NCI13</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - NCI14</t>
+  </si>
+  <si>
+    <t>Subsidiaries (at cost) - A</t>
+  </si>
+  <si>
+    <t>Investment property (at cost) - B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shares/Bonds (at cost/unlisted) - C</t>
+  </si>
+  <si>
+    <t>Other investments (at cost) - D</t>
+  </si>
+  <si>
+    <t>Investment property (at FV) - E</t>
+  </si>
+  <si>
+    <t>Managed funds (at FV) - F</t>
+  </si>
+  <si>
+    <t>Cash deposits (at FV) - G</t>
+  </si>
+  <si>
+    <t>Shares/Bonds (at FV/listed) - H</t>
+  </si>
+  <si>
+    <t>Other investments (at FV) - I</t>
+  </si>
+  <si>
+    <t>Total  - J</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance Return(£000) - CUI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - CUI2</t>
+  </si>
+  <si>
+    <t>Additions (£000) - CUI3</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - CUI4</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - CUI5</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - CUI6</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - CUI7</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - CUI8</t>
+  </si>
+  <si>
+    <t>Impairments (£000) - CUI9</t>
+  </si>
+  <si>
+    <t>Reclassification from non-current asset investments (£000) - CUI10</t>
+  </si>
+  <si>
+    <t>Reclassification to non-current asset investments (£000) - CUI11</t>
+  </si>
+  <si>
+    <t>Reclassification within current asset investments (£000) - CUI12</t>
+  </si>
+  <si>
+    <t>Period end fair value gain/(loss) (£000) - CUI13</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - CUI14</t>
+  </si>
+  <si>
+    <t>Total - J</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - TFC1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - TFC2</t>
+  </si>
+  <si>
+    <t>Additions - funded from Free Schools/Priority Schools Building programme (£000) - TFC3</t>
+  </si>
+  <si>
+    <t>Additions - funded from other DFE and ESFA (EFA) capital grant (£000) - TFC4</t>
+  </si>
+  <si>
+    <t>Additions - other (£000) - TFC5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - TFC6</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - TFC7</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - TFC8</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - TFC9</t>
+  </si>
+  <si>
+    <t>Donations (DFE and ESFA (EFA)) (£000) - TFC10</t>
+  </si>
+  <si>
+    <t>Donations (non-DFE and ESFA (EFA)) (£000) - TFC11</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - TFC12</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - TFC13</t>
+  </si>
+  <si>
+    <t>Valuation adjustment (£000) - TFC14</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - TFC15</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - TFC16</t>
+  </si>
+  <si>
+    <t>Freehold Land and Buildings - A</t>
+  </si>
+  <si>
+    <t>Leasehold Land and Buildings - B</t>
+  </si>
+  <si>
+    <t>Leasehold Improvements - C</t>
+  </si>
+  <si>
+    <t>Plant and Machinery - D</t>
+  </si>
+  <si>
+    <t>Furniture and Equipment - E</t>
+  </si>
+  <si>
+    <t>Computer Equipment - F</t>
+  </si>
+  <si>
+    <t>Motor Vehicles - G</t>
+  </si>
+  <si>
+    <t>Assets under construction - H</t>
+  </si>
+  <si>
+    <t>Total - I</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - TFD1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - TFD2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - TFD3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - TFD4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - TFD5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - TFD6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - TFD7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - TFD8</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - TFD9</t>
+  </si>
+  <si>
+    <t>Leasehold land and Buildings - B</t>
+  </si>
+  <si>
+    <t>Total - H</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - TFI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - TFI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - TFI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - TFI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - TFI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - TFI6</t>
+  </si>
+  <si>
+    <t>Closing Balance (£000) - TFI7</t>
+  </si>
+  <si>
+    <t>Furniture &amp; Equipment - E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Motor Vehicles - G</t>
+  </si>
+  <si>
+    <t>Freehold land and buildings (£000) - TFV1</t>
+  </si>
+  <si>
+    <t>Leasehold land and buildings (£000) - TFV2</t>
+  </si>
+  <si>
+    <t>Leasehold improvements (£000) - TFI3</t>
+  </si>
+  <si>
+    <t>Plant and machinery (£000) - TFI4</t>
+  </si>
+  <si>
+    <t>Furniture and equipment (£000) - TFI5</t>
+  </si>
+  <si>
+    <t>Computer equipment (£000) - TFI6</t>
+  </si>
+  <si>
+    <t>Motor vehicles (£000) - TFI7</t>
+  </si>
+  <si>
+    <t>Assets under construction (£000) - TFI8</t>
+  </si>
+  <si>
+    <t>Total (£000) - TFI9</t>
+  </si>
+  <si>
+    <t>Owned (£000) - TFF1</t>
+  </si>
+  <si>
+    <t>Finance leased (£000) - TFF2</t>
+  </si>
+  <si>
+    <t>Other(£000) - TFF3</t>
+  </si>
+  <si>
+    <t>On-balance sheet PFI contracts (£000) - TFF4</t>
+  </si>
+  <si>
+    <t>Total (£000) - TFF5</t>
+  </si>
+  <si>
+    <t>Plant &amp; Machinery - D</t>
+  </si>
+  <si>
+    <t>Single period or minimum of range (months) - DP1</t>
+  </si>
+  <si>
+    <t>Maximum of range (months) - DP2</t>
+  </si>
+  <si>
+    <t>Reducing balance rate (%) - DP3</t>
+  </si>
+  <si>
+    <t>Trade debtors before bad debt (£000) - DE1</t>
+  </si>
+  <si>
+    <t>Bad debts (£000)  - DE2</t>
+  </si>
+  <si>
+    <t>Accrued capital grant DfE/ESFA (£000) - DE3</t>
+  </si>
+  <si>
+    <t>Accrued capital grant - other (£000) - DE4</t>
+  </si>
+  <si>
+    <t>Accrued revenue grants DFE/ESFA (£000) - DE5</t>
+  </si>
+  <si>
+    <t>Accrued revenue grants - other (£000) - DE6</t>
+  </si>
+  <si>
+    <t>Prepayments (£000) - DE7</t>
+  </si>
+  <si>
+    <t>Amount due within 1 year - A</t>
+  </si>
+  <si>
+    <t>Amount due after 1 year - B</t>
+  </si>
+  <si>
+    <t>Stock - S1</t>
+  </si>
+  <si>
+    <t>Cash balance (£000) - C1</t>
+  </si>
+  <si>
+    <t>Condition Improvement Fund (CIF) (£000) - AG1</t>
+  </si>
+  <si>
+    <t>MATs School Condition Allowance (SCA) (£000) - AG2</t>
+  </si>
+  <si>
+    <t>Priority School Building Programme (PSBP) (£000) - AG3</t>
+  </si>
+  <si>
+    <t>Devolved Formula Capital Grant (DFC) (£000) - AG4</t>
+  </si>
+  <si>
+    <t>Centrally Managed Programme - Free Schools (£000) - AG5</t>
+  </si>
+  <si>
+    <t>Continuing Commitments - Building Schools for the Future (BSF) (£000) - AG6</t>
+  </si>
+  <si>
+    <t>Schools Sponsorship Development Fund (SSDF) (£000) - AG7</t>
+  </si>
+  <si>
+    <t>Other (£000) - AG8</t>
+  </si>
+  <si>
+    <t>Local Authority Capital Grants (£000) - AG9</t>
+  </si>
+  <si>
+    <t>Other Government Capital Grants (£000) - AG10</t>
+  </si>
+  <si>
+    <t>Non-Government Capital Grants (£000) - AG11</t>
+  </si>
+  <si>
+    <t>Total (£000) - AG12</t>
+  </si>
+  <si>
+    <t>Donation fixed assets (non DFE/ESFA) (£000) - AD1</t>
+  </si>
+  <si>
+    <t>Fixed assets donated by the DFE/ESFA (£000) - AD2</t>
+  </si>
+  <si>
+    <t>Donated intangible assets (£000) - AD3</t>
+  </si>
+  <si>
+    <t>Other donations (£000) - AD4</t>
+  </si>
+  <si>
+    <t>Total (£000) - AD5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority  (£000) - AT1</t>
+  </si>
+  <si>
+    <t>Transferred in on existing academies joining the trust (£000) - AT2</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - AT3</t>
+  </si>
+  <si>
+    <t>Total (£000) - AT4</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance as submitted in the Accounts Return (£000) - AFC1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - AFC2</t>
+  </si>
+  <si>
+    <t>Additions - funded from Free Schools/Priority Schools Building programme (£000) - AFC3</t>
+  </si>
+  <si>
+    <t>Additions - funded from other DFE/ESFA capital grant (£000) - AFC4</t>
+  </si>
+  <si>
+    <t>Additions - other (£000) - AFC5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - AFC6</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - AFC7</t>
+  </si>
+  <si>
+    <t>Transferred in on existing academies joining the trust (£000) - AFC8</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - AFC9</t>
+  </si>
+  <si>
+    <t>Donations (DFE/ESFA) (£000) - AFC10</t>
+  </si>
+  <si>
+    <t>Donations (non-DFE/ESFA) (£000) - AFC11</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - AFC12</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - AFC13</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - AFC14</t>
+  </si>
+  <si>
+    <t>Total closing balance - AFC15</t>
+  </si>
+  <si>
+    <t>Freehold Land &amp; Buildings - A</t>
+  </si>
+  <si>
+    <t>Leasehold Land &amp; Buildings - B</t>
+  </si>
+  <si>
+    <t>Leasehold improvements - C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Furniture &amp; Equipment - </t>
+  </si>
+  <si>
+    <t>Assets under construction - G</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance as submitted in the Accounts Return (£000) - AFD1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - AFD2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - AFD3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - AFD4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing academies joining the trust (£000) - AFD5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - AFD6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - AFD7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - AFD8</t>
+  </si>
+  <si>
+    <t>Total closing balance - AFD9</t>
+  </si>
+  <si>
+    <t>Assets under constructions - G</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance as submitted in the Accounts Return (£000) - AFI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - AFI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - AFI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - AFI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing academies joining the trust (£000) - AFI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - AFI6</t>
+  </si>
+  <si>
+    <t>Total closing balance - AFI7</t>
+  </si>
+  <si>
+    <t>Accrued capital grant DFE/ESFA (£000) - ADE1</t>
+  </si>
+  <si>
+    <t>Accrued capital grant - other (£000) - ADE2</t>
+  </si>
+  <si>
+    <t>Accrued income (£000) - ADE3</t>
+  </si>
+  <si>
+    <t>Other debtors (£000) - ADE4</t>
+  </si>
+  <si>
+    <t>Total (£000) - ADE5</t>
+  </si>
+  <si>
+    <t>Amounts due within 1 year - A</t>
+  </si>
+  <si>
+    <t>Amounts due after more than 1 year - B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refering not provided in specificaltion </t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LTC1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LTC2</t>
+  </si>
+  <si>
+    <t>Additions - funded from Free Schools/Priority Schools Building programme (£000) - LTC3</t>
+  </si>
+  <si>
+    <t>Additions - funded from other DFE and ESFA (EFA) capital grant (£000) - LTC4</t>
+  </si>
+  <si>
+    <t>Additions - other (£000) - LTC5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - LTC6</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - LTC7</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LTC8</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - LTC9</t>
+  </si>
+  <si>
+    <t>Donations (DFE and ESFA (EFA)) (£000) - LTC10</t>
+  </si>
+  <si>
+    <t>Donations (non-DFE and ESFA (EFA)) (£000) - LTC11</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - LTC12</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LTC13</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LTC14</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LTC15</t>
+  </si>
+  <si>
+    <t>Assets under construction - D</t>
+  </si>
+  <si>
+    <t>Total - E</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LTD1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LTD2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LTD3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - LTD4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LTD5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LTD6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LTD7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LTD8</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LTD9</t>
+  </si>
+  <si>
+    <t>Total - D</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LTI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LTI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LTI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - LTI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies leaving the Trust (£000) - LTI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LTI6</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LTI7</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LAC1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LAC2</t>
+  </si>
+  <si>
+    <t>Additions - funded from Free Schools/Priority Schools Building programme (£000) - LAC3</t>
+  </si>
+  <si>
+    <t>Additions - funded from other DFE and ESFA (EFA) capital grant (£000) - LAC4</t>
+  </si>
+  <si>
+    <t>Additions - other (£000) - LAC5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - LAC6</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - LAC7</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LAC8</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - LAC9</t>
+  </si>
+  <si>
+    <t>Donations (DFE and ESFA (EFA)) (£000) - LAC10</t>
+  </si>
+  <si>
+    <t>Donations (non-DFE and ESFA (EFA)) (£000) - LAC11</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - LAC12</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LAC13</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LAC14</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LAC15</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LAD1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LAD2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LAD3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - LAD4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LAD5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LAD6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LAD7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LAD8</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LAD9</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LAI1</t>
+  </si>
+  <si>
+    <t>Adjustments made to opening balance (£000) - LAI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LAI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - LAI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies leaving the Trust (£000) - LAI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LAI6</t>
+  </si>
+  <si>
+    <t>Closing Balance (£000) - LAI7</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LLC1</t>
+  </si>
+  <si>
+    <t>Other Adjustments made to opening balance (£000) - LLC2</t>
+  </si>
+  <si>
+    <t>Additions - funded from Free Schools/Priority Schools Building programme (£000) - LLC3</t>
+  </si>
+  <si>
+    <t>Additions - funded from other DFE and ESFA (EFA) capital grant (£000) - LLC4</t>
+  </si>
+  <si>
+    <t>Additions - other (£000) - LLC5</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - local authority (£000) - LLC6</t>
+  </si>
+  <si>
+    <t>Transferred in on conversion - elsewhere (£000) - LLC7</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LLC8</t>
+  </si>
+  <si>
+    <t>Transferred out on existing Academies leaving the Trust (£000) - LLC9</t>
+  </si>
+  <si>
+    <t>Donations (DFE and ESFA (EFA)) (£000) - LLC10</t>
+  </si>
+  <si>
+    <t>Donations (non-DFE and ESFA (EFA)) (£000) - LLC11</t>
+  </si>
+  <si>
+    <t>Disposals (£000) - LLC12</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LLC13</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LLC14</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LLC15</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LLD1</t>
+  </si>
+  <si>
+    <t>Other Adjustments made to opening balance (£000) - LLD2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LLD3</t>
+  </si>
+  <si>
+    <t>Eliminated on disposal (£000) - LLD4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies joining the Trust (£000) - LLD5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LLD6</t>
+  </si>
+  <si>
+    <t>Revaluations (£000) - LLD7</t>
+  </si>
+  <si>
+    <t>Reclassifications (£000) - LLD8</t>
+  </si>
+  <si>
+    <t>At close of period (£000) - LLD9</t>
+  </si>
+  <si>
+    <t>Original prior year closing balance (£000) - LLI1</t>
+  </si>
+  <si>
+    <t>Other Adjustments made to opening balance (£000) - LLI2</t>
+  </si>
+  <si>
+    <t>Charged in period (£000) - LLI3</t>
+  </si>
+  <si>
+    <t>Released in period (£000) - LLI4</t>
+  </si>
+  <si>
+    <t>Transferred in on existing Academies leaving the Trust (£000) - LLI5</t>
+  </si>
+  <si>
+    <t>Transferred out on existing academies leaving the trust (£000) - LLI6</t>
+  </si>
+  <si>
+    <t>Closing Balance (£000) - LLI7</t>
+  </si>
+  <si>
+    <t>Net book value - LLV1</t>
   </si>
 </sst>
 </file>
@@ -922,7 +1902,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ ;[Red]\(#,##0\);\ \-\ \ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1013,6 +1993,30 @@
       <name val="Andale Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Andale Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1094,7 +2098,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1138,6 +2142,35 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -19263,7 +20296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -19344,6 +20377,356 @@
         <v>28</v>
       </c>
       <c r="D12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>326</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19491,6 +20874,947 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="27" t="s">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="58.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
@@ -19532,6 +21856,774 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="91.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="103.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="103.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>504</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>522</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -19646,6 +22738,626 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>602</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>522</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>522</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>522</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Referencing update : Staff Costs.
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33580" yWindow="800" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="s_Donations" sheetId="1" r:id="rId1"/>
@@ -6273,9 +6273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6481,7 +6479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testing References for IFA Impairments page
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="20" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="s_Donations" sheetId="1" r:id="rId1"/>
@@ -6273,7 +6273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7245,13 +7245,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Testing the Land and Buildings Trust Owned Depreciation Page FF
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="20" activeTab="24"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="39" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="s_Donations" sheetId="1" r:id="rId1"/>
@@ -7245,7 +7245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7429,7 +7429,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8719,8 +8719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Land and building : Academies Cost , Depreciation and Impairments.
</commit_message>
<xml_diff>
--- a/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
+++ b/src/test/dataSheetsResources/AR_DataSheet/AR3_DataSheetReferences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="39" activeTab="42"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500" firstSheet="53" activeTab="62"/>
   </bookViews>
   <sheets>
     <sheet name="s_Donations" sheetId="1" r:id="rId1"/>
@@ -8719,7 +8719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -10407,8 +10407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>